<commit_message>
updated payless test cases
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Anonymous.xlsx
+++ b/budget-web-tests/testData/Anonymous.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215"/>
+    <workbookView windowWidth="23040" windowHeight="11148"/>
   </bookViews>
   <sheets>
     <sheet name="Anonymous" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="106">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Budget_RES_U_type Coupon_PayLater_US</t>
   </si>
   <si>
-    <t>EWR</t>
-  </si>
-  <si>
     <t>UUZZ011</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
   </si>
   <si>
     <t>Budget_RES_G_typeCoupon__SMSCheckbox_IATA_PayLater_US</t>
-  </si>
-  <si>
-    <t>GUZZ007</t>
   </si>
   <si>
     <t>Budget_RES _Digital wallet Uplift _Direct_modify flow_US</t>
@@ -346,11 +340,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -374,7 +368,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -382,23 +376,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,22 +414,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,22 +422,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,22 +438,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -490,7 +445,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,6 +484,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,13 +520,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,19 +550,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,19 +592,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,49 +616,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,7 +640,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,49 +682,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -724,25 +718,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,36 +734,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -809,6 +755,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -817,15 +772,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -834,136 +831,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -977,7 +971,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1311,12 +1305,14 @@
   <dimension ref="A1:BA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:BA21"/>
+      <selection activeCell="B24" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="24.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="64.4444444444444" customWidth="1"/>
+    <col min="33" max="33" width="9.22222222222222"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53">
@@ -1642,7 +1638,7 @@
       </c>
     </row>
     <row r="3" spans="1:53">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1803,7 +1799,7 @@
       </c>
     </row>
     <row r="4" spans="1:53">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1964,7 +1960,7 @@
       </c>
     </row>
     <row r="5" spans="1:53">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2125,7 +2121,7 @@
       </c>
     </row>
     <row r="6" spans="1:53">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2286,7 +2282,7 @@
       </c>
     </row>
     <row r="7" spans="1:53">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2447,7 +2443,7 @@
       </c>
     </row>
     <row r="8" spans="1:53">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2608,7 +2604,7 @@
       </c>
     </row>
     <row r="9" spans="1:53">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2769,7 +2765,7 @@
       </c>
     </row>
     <row r="10" spans="1:53">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2930,7 +2926,7 @@
       </c>
     </row>
     <row r="11" spans="1:53">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2946,28 +2942,28 @@
         <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>56</v>
@@ -3091,11 +3087,11 @@
       </c>
     </row>
     <row r="12" spans="1:53">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>55</v>
@@ -3252,11 +3248,11 @@
       </c>
     </row>
     <row r="13" spans="1:53">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>55</v>
@@ -3413,11 +3409,11 @@
       </c>
     </row>
     <row r="14" spans="1:53">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>55</v>
@@ -3441,7 +3437,7 @@
         <v>56</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>56</v>
@@ -3574,11 +3570,11 @@
       </c>
     </row>
     <row r="15" spans="1:53">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
@@ -3596,25 +3592,25 @@
         <v>56</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>56</v>
@@ -3735,11 +3731,11 @@
       </c>
     </row>
     <row r="16" spans="1:53">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>55</v>
@@ -3751,7 +3747,7 @@
         <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>56</v>
@@ -3896,11 +3892,11 @@
       </c>
     </row>
     <row r="17" spans="1:53">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
@@ -4057,11 +4053,11 @@
       </c>
     </row>
     <row r="18" spans="1:53">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>55</v>
@@ -4079,13 +4075,13 @@
         <v>56</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>56</v>
@@ -4094,7 +4090,7 @@
         <v>56</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>56</v>
@@ -4218,11 +4214,11 @@
       </c>
     </row>
     <row r="19" spans="1:53">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>55</v>
@@ -4379,11 +4375,11 @@
       </c>
     </row>
     <row r="20" spans="1:53">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>55</v>
@@ -4540,11 +4536,11 @@
       </c>
     </row>
     <row r="21" spans="1:53">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>55</v>
@@ -4881,7 +4877,7 @@
     <row r="2" spans="1:53">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
budget CA test cases
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Anonymous.xlsx
+++ b/budget-web-tests/testData/Anonymous.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/web_migration_updated 14 march/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B67F03F-22CA-064D-A1A2-D4DF59CC60D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F70ABC7-1601-014D-9734-5425C5D074A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anonymous" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="122">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -351,6 +351,42 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>YYZ</t>
+  </si>
+  <si>
+    <t>British Columbia</t>
+  </si>
+  <si>
+    <t>L4M0A4</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Budget_RES_Inbound_MultiCurrency_IATA_Cancellation_PayNow_CA</t>
+  </si>
+  <si>
+    <t>Budget_RES_Outbound_USAA_Validate_CorpBooking_CA</t>
+  </si>
+  <si>
+    <t>Budget_RES_Modify/cancel flow_Step1_to_Step4_CA</t>
+  </si>
+  <si>
+    <t>Budget_RES_Domestic_PayLater_CA</t>
+  </si>
+  <si>
+    <t>Budget_RES_Incognito_PayLater_CA</t>
+  </si>
+  <si>
+    <t>Budget_RES_KeyDropLocation_M_typeCoupon_PayLater_CA</t>
+  </si>
+  <si>
+    <t>YYC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SFO </t>
   </si>
 </sst>
 </file>
@@ -360,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +437,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -419,12 +463,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -447,8 +494,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC21"/>
+  <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AT28" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -906,9 +956,7 @@
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" t="s">
         <v>54</v>
       </c>
@@ -1073,9 +1121,7 @@
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -1240,9 +1286,7 @@
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>69</v>
       </c>
@@ -1407,9 +1451,7 @@
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>71</v>
       </c>
@@ -1574,9 +1616,7 @@
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -1741,9 +1781,7 @@
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -1908,9 +1946,7 @@
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -2075,9 +2111,7 @@
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>82</v>
       </c>
@@ -2242,9 +2276,7 @@
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>84</v>
       </c>
@@ -2409,9 +2441,7 @@
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>87</v>
       </c>
@@ -2576,9 +2606,7 @@
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>89</v>
       </c>
@@ -2743,9 +2771,7 @@
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>90</v>
       </c>
@@ -2910,9 +2936,7 @@
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>91</v>
       </c>
@@ -3077,9 +3101,7 @@
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>93</v>
       </c>
@@ -3244,9 +3266,7 @@
       </c>
     </row>
     <row r="16" spans="1:55" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
@@ -3411,9 +3431,7 @@
       </c>
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>98</v>
       </c>
@@ -3578,9 +3596,7 @@
       </c>
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>99</v>
       </c>
@@ -3745,9 +3761,7 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>100</v>
       </c>
@@ -3912,9 +3926,7 @@
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>105</v>
       </c>
@@ -4079,9 +4091,7 @@
       </c>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>98</v>
       </c>
@@ -4245,7 +4255,1012 @@
         <v>56</v>
       </c>
     </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V22" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W22" s="8">
+        <v>342000000000000</v>
+      </c>
+      <c r="X22" s="6">
+        <v>1129</v>
+      </c>
+      <c r="Y22" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z22" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB22" s="6">
+        <v>123</v>
+      </c>
+      <c r="AC22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V23" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG23" s="6">
+        <v>38298026</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC23" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V24" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X24" s="6">
+        <v>1129</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB24" s="6">
+        <v>123</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE24" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC24" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V25" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC25" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V26" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC26" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I27" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S27" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V27" s="8">
+        <v>9840000000</v>
+      </c>
+      <c r="W27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC27" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AN22" r:id="rId1" display="mailto:test@munters.com" xr:uid="{43FBD047-67B5-4244-8EF0-E4FA0747AE15}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Budget US test cases
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Anonymous.xlsx
+++ b/budget-web-tests/testData/Anonymous.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Downloads/web_framework_updated branch 16 march/ecom-us-web/budget-web-tests/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/web_framework_updated 20 march/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B97CD1-AE5B-454D-9748-BB3A7D52A3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED358F9A-765F-0D48-8F9B-22D17F59D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Anonymous" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Authenticated" sheetId="2" r:id="rId3"/>
+    <sheet name="Budget US Anonymous" sheetId="1" r:id="rId1"/>
+    <sheet name="Budget CA Anonymous" sheetId="3" r:id="rId2"/>
+    <sheet name="Budget NZ Anonymous" sheetId="4" r:id="rId3"/>
+    <sheet name="Authenticated" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="141">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -430,6 +431,21 @@
   </si>
   <si>
     <t>YUL</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Domestic_Anonymous_PayLater_NZ</t>
+  </si>
+  <si>
+    <t>COR</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Inbound_PayLater_NZ</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Outbound_PayLater_NZ</t>
+  </si>
+  <si>
+    <t>Budget_Reservation_Domestic_PayNow_NZ</t>
   </si>
 </sst>
 </file>
@@ -440,12 +456,19 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -511,39 +534,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -822,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:BC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -936,7 +962,7 @@
       <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
       <c r="AH1" t="s">
@@ -1007,7 +1033,9 @@
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
@@ -1172,8 +1200,10 @@
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C3" t="s">
@@ -1337,7 +1367,9 @@
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
@@ -1502,7 +1534,9 @@
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B5" t="s">
         <v>71</v>
       </c>
@@ -1667,7 +1701,9 @@
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -1832,7 +1868,9 @@
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -1997,7 +2035,9 @@
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -2162,7 +2202,9 @@
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B9" t="s">
         <v>82</v>
       </c>
@@ -2327,7 +2369,9 @@
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B10" t="s">
         <v>84</v>
       </c>
@@ -2492,7 +2536,9 @@
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B11" t="s">
         <v>87</v>
       </c>
@@ -2657,7 +2703,9 @@
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>89</v>
       </c>
@@ -2822,7 +2870,9 @@
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B13" t="s">
         <v>90</v>
       </c>
@@ -2987,7 +3037,9 @@
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B14" t="s">
         <v>91</v>
       </c>
@@ -3152,7 +3204,9 @@
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B15" t="s">
         <v>93</v>
       </c>
@@ -3317,7 +3371,9 @@
       </c>
     </row>
     <row r="16" spans="1:55" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B16" s="4" t="s">
         <v>97</v>
       </c>
@@ -3482,7 +3538,9 @@
       </c>
     </row>
     <row r="17" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B17" t="s">
         <v>98</v>
       </c>
@@ -3647,7 +3705,9 @@
       </c>
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B18" t="s">
         <v>99</v>
       </c>
@@ -3812,7 +3872,9 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B19" t="s">
         <v>100</v>
       </c>
@@ -3977,7 +4039,9 @@
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B20" s="4" t="s">
         <v>105</v>
       </c>
@@ -4142,7 +4206,9 @@
       </c>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B21" t="s">
         <v>98</v>
       </c>
@@ -4347,8 +4413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F8B337-C646-F645-8F2E-76CD5765FF7A}">
   <dimension ref="A1:BC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4525,9 +4591,7 @@
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="6" t="s">
         <v>118</v>
       </c>
@@ -4692,9 +4756,7 @@
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A3" s="4"/>
       <c r="B3" s="6" t="s">
         <v>116</v>
       </c>
@@ -4859,9 +4921,7 @@
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" s="6" t="s">
         <v>119</v>
       </c>
@@ -5026,9 +5086,7 @@
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>122</v>
       </c>
@@ -5119,7 +5177,7 @@
       <c r="AE5" t="s">
         <v>56</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AG5" s="3">
@@ -5193,9 +5251,7 @@
       </c>
     </row>
     <row r="6" spans="1:55" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
         <v>114</v>
       </c>
@@ -5360,9 +5416,7 @@
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
         <v>115</v>
       </c>
@@ -5527,9 +5581,7 @@
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" s="6" t="s">
         <v>121</v>
       </c>
@@ -5694,9 +5746,7 @@
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="4"/>
       <c r="B9" s="6" t="s">
         <v>117</v>
       </c>
@@ -5861,9 +5911,7 @@
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>123</v>
       </c>
@@ -6028,9 +6076,7 @@
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>124</v>
       </c>
@@ -6195,9 +6241,7 @@
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
         <v>125</v>
       </c>
@@ -6362,9 +6406,7 @@
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>126</v>
       </c>
@@ -6529,9 +6571,7 @@
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>127</v>
       </c>
@@ -6696,9 +6736,7 @@
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>128</v>
       </c>
@@ -6863,9 +6901,7 @@
       </c>
     </row>
     <row r="16" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>129</v>
       </c>
@@ -7030,9 +7066,7 @@
       </c>
     </row>
     <row r="17" spans="1:55" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>130</v>
       </c>
@@ -7197,9 +7231,7 @@
       </c>
     </row>
     <row r="18" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>117</v>
       </c>
@@ -7364,9 +7396,7 @@
       </c>
     </row>
     <row r="19" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>131</v>
       </c>
@@ -7531,9 +7561,7 @@
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>132</v>
       </c>
@@ -7698,9 +7726,7 @@
       </c>
     </row>
     <row r="21" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>133</v>
       </c>
@@ -7876,6 +7902,693 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F8901E-2144-8541-8BFC-719A0D3FE47B}">
+  <dimension ref="A1:BC5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="45.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" s="11">
+        <v>9840000000</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC2" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="10">
+        <v>9838234567</v>
+      </c>
+      <c r="W3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC3" s="6">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="10">
+        <v>9838234567</v>
+      </c>
+      <c r="W4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC4" s="6">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BA2"/>
   <sheetViews>

</xml_diff>